<commit_message>
Day 1: Added catering project intro + notes update
</commit_message>
<xml_diff>
--- a/03_Notes/learning_tracker.xlsx.xlsx
+++ b/03_Notes/learning_tracker.xlsx.xlsx
@@ -172,9 +172,6 @@
 </t>
   </si>
   <si>
-    <t>created backend journey folder structure</t>
-  </si>
-  <si>
     <t>1. How to run python
 2. how to use vs code
 3. how to connect github
@@ -191,8 +188,12 @@
     <t>4 hours</t>
   </si>
   <si>
-    <t>mani.py
-project folders created</t>
+    <t>Created project base structure
+Initialized project intro file</t>
+  </si>
+  <si>
+    <t>main.py
+project_intro.py</t>
   </si>
 </sst>
 </file>
@@ -546,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +696,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="225" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>46063</v>
       </c>
@@ -721,22 +722,22 @@
         <v>26</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O4" s="2">
         <v>6</v>

</xml_diff>